<commit_message>
added mech design temp finder func
</commit_message>
<xml_diff>
--- a/whb_tubewall/input_from_gips.xlsx
+++ b/whb_tubewall/input_from_gips.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{B1122066-076A-41B3-B045-0C739043DE87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E9BD9F2-8C56-45E0-B7A7-3506D7D18A4D}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="8_{B1122066-076A-41B3-B045-0C739043DE87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93CF6BBF-96B5-4CBD-9F04-57745957982A}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31716" yWindow="3384" windowWidth="19092" windowHeight="11556" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -383,7 +383,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -421,7 +421,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="1">
-        <v>31.75</v>
+        <v>38.1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -432,7 +432,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="1">
-        <v>21.43</v>
+        <v>23.68</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="28" x14ac:dyDescent="0.3">
@@ -443,7 +443,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="1">
-        <v>6</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="28" x14ac:dyDescent="0.3">
@@ -454,7 +454,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="1">
-        <v>1111</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="28" x14ac:dyDescent="0.3">
@@ -465,7 +465,7 @@
         <v>9</v>
       </c>
       <c r="C7" s="1">
-        <v>20230.660400000001</v>
+        <v>21495.606500000002</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -476,7 +476,7 @@
         <v>11</v>
       </c>
       <c r="C8" s="1">
-        <v>475</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -487,7 +487,7 @@
         <v>11</v>
       </c>
       <c r="C9" s="1">
-        <v>350</v>
+        <v>474</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="42" x14ac:dyDescent="0.3">
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="C10" s="1">
-        <v>8.7420000000000009</v>
+        <v>8.6898999999999997</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="28" x14ac:dyDescent="0.3">
@@ -509,7 +509,7 @@
         <v>14</v>
       </c>
       <c r="C11" s="1">
-        <v>7.7483000000000004</v>
+        <v>7.7099000000000002</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="42" x14ac:dyDescent="0.3">
@@ -520,7 +520,7 @@
         <v>17</v>
       </c>
       <c r="C12" s="1">
-        <v>49010.786800000002</v>
+        <v>110654.9954</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="28" x14ac:dyDescent="0.3">
@@ -531,7 +531,7 @@
         <v>17</v>
       </c>
       <c r="C13" s="1">
-        <v>15757.168799999999</v>
+        <v>37410.1999</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="56" x14ac:dyDescent="0.3">
@@ -542,7 +542,7 @@
         <v>17</v>
       </c>
       <c r="C14" s="1">
-        <v>767.70719999999994</v>
+        <v>642.16989999999998</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="28" x14ac:dyDescent="0.3">
@@ -553,7 +553,7 @@
         <v>17</v>
       </c>
       <c r="C15" s="1">
-        <v>722.3537</v>
+        <v>514.86440000000005</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="42" x14ac:dyDescent="0.3">
@@ -564,7 +564,7 @@
         <v>11</v>
       </c>
       <c r="C16" s="1">
-        <v>327.20299999999997</v>
+        <v>324.68610000000001</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="42" x14ac:dyDescent="0.3">
@@ -575,7 +575,7 @@
         <v>21</v>
       </c>
       <c r="C17" s="1">
-        <v>4.3155999999999999</v>
+        <v>3.8203</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="28" x14ac:dyDescent="0.3">
@@ -586,7 +586,7 @@
         <v>23</v>
       </c>
       <c r="C18" s="1">
-        <v>12.9413</v>
+        <v>13.1989</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="42" x14ac:dyDescent="0.3">
@@ -597,7 +597,7 @@
         <v>25</v>
       </c>
       <c r="C19" s="1">
-        <v>4.53E-2</v>
+        <v>4.5499999999999999E-2</v>
       </c>
     </row>
   </sheetData>
@@ -607,21 +607,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<TemplafyTemplateConfiguration><![CDATA[{"transformationConfigurations":[{"colorTheme":"{{UserProfile.Location.ColorThemeRef.ColorTheme}}","disableUpdates":false,"type":"colorTheme"}],"templateName":"Blank","templateDescription":"","enableDocumentContentUpdater":true,"version":"2.0"}]]></TemplafyTemplateConfiguration>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <TemplafyFormConfiguration><![CDATA[{"formFields":[],"formDataEntries":[]}]]></TemplafyFormConfiguration>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<TemplafyTemplateConfiguration><![CDATA[{"transformationConfigurations":[{"colorTheme":"{{UserProfile.Location.ColorThemeRef.ColorTheme}}","disableUpdates":false,"type":"colorTheme"}],"templateName":"Blank","templateDescription":"","enableDocumentContentUpdater":true,"version":"2.0"}]]></TemplafyTemplateConfiguration>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34ECD078-1A11-477F-8080-F9D902BF81D7}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{904BC371-2ADF-4271-BF15-7D239A4D7695}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34ECD078-1A11-477F-8080-F9D902BF81D7}">
-  <ds:schemaRefs/>
-</ds:datastoreItem>
 </file>
</xml_diff>